<commit_message>
Framework Design , added testng.xml
</commit_message>
<xml_diff>
--- a/RestAssuredMainAssignment/src/test/data/Add20Task.xlsx
+++ b/RestAssuredMainAssignment/src/test/data/Add20Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HUAPI\RestAssuredMainAssignment\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6ACDED1-9FA1-4787-91A5-B2548BA9CA53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516F7362-9A23-4FCC-A42B-5768A746AFF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="6">
   <si>
     <t>description</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>eating</t>
+  </si>
+  <si>
+    <t>swimming</t>
   </si>
 </sst>
 </file>
@@ -429,6 +432,9 @@
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">

</xml_diff>